<commit_message>
Change 2 Ohm Resistor
Had to change for heatsink mounting :/
</commit_message>
<xml_diff>
--- a/RLOOP_BMS_V2/rLoopBMSv2 BOM.xlsx
+++ b/RLOOP_BMS_V2/rLoopBMSv2 BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="rLoopBMSv2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Reference</t>
   </si>
@@ -58,9 +58,6 @@
     <t>EL-17-21VGC/TR8</t>
   </si>
   <si>
-    <t>MP930-2.00-1%</t>
-  </si>
-  <si>
     <t>PMV20ENR</t>
   </si>
   <si>
@@ -164,6 +161,15 @@
   </si>
   <si>
     <t>SMF6.5A / SOD-123</t>
+  </si>
+  <si>
+    <t>Heatsink: 542502B00000G x16</t>
+  </si>
+  <si>
+    <t>Fanx: 2x 0D7025-24MB x2</t>
+  </si>
+  <si>
+    <t>TBH25P2R00JE</t>
   </si>
 </sst>
 </file>
@@ -985,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1008,7 +1014,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1016,15 +1022,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -1032,7 +1038,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1040,15 +1046,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1056,7 +1062,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -1064,26 +1070,26 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1096,10 +1102,10 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1112,7 +1118,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -1120,31 +1126,31 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -1152,7 +1158,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1160,42 +1166,52 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
         <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
         <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
-        <v>21</v>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>